<commit_message>
added some p values
</commit_message>
<xml_diff>
--- a/output/bigexcel.xlsx
+++ b/output/bigexcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victoria/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saqin\Desktop\Something_Cool-CpG_Sites-\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33785C67-4F08-D849-9B7A-BD5DFAF66135}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7D1CB2-0788-49A5-9DE6-9B18DF9F3D99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="460" windowWidth="27640" windowHeight="15960" xr2:uid="{8D3C0EB5-B848-6042-B945-4E985C0A2D75}"/>
+    <workbookView xWindow="4215" yWindow="465" windowWidth="27645" windowHeight="15960" xr2:uid="{8D3C0EB5-B848-6042-B945-4E985C0A2D75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="58">
   <si>
     <t>File</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>Costly: T-&gt;C Syn</t>
+  </si>
+  <si>
+    <t>&lt;0.01</t>
   </si>
 </sst>
 </file>
@@ -596,16 +599,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFE611C-6421-1741-B53C-4075AD299B10}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -643,7 +646,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -656,6 +659,24 @@
       <c r="D2" t="s">
         <v>53</v>
       </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
       <c r="K2">
         <v>2.2271225403678701</v>
       </c>
@@ -663,7 +684,7 @@
         <v>2.3633695171438802</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -676,6 +697,24 @@
       <c r="D3" t="s">
         <v>53</v>
       </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>57</v>
+      </c>
       <c r="K3">
         <v>1.38769839128198</v>
       </c>
@@ -683,7 +722,7 @@
         <v>1.6836081856637899</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -696,6 +735,24 @@
       <c r="D4" t="s">
         <v>53</v>
       </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4">
+        <v>2.2700000000000001E-2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" t="s">
+        <v>57</v>
+      </c>
       <c r="K4">
         <v>1.69459448388228</v>
       </c>
@@ -703,7 +760,7 @@
         <v>2.8369452622121298</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -716,6 +773,24 @@
       <c r="D5" t="s">
         <v>53</v>
       </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J5" t="s">
+        <v>57</v>
+      </c>
       <c r="K5">
         <v>1.90734628459693</v>
       </c>
@@ -723,7 +798,7 @@
         <v>2.31957942082171</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -736,6 +811,24 @@
       <c r="D6" t="s">
         <v>53</v>
       </c>
+      <c r="E6">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6">
+        <v>2.3699999999999999E-2</v>
+      </c>
+      <c r="I6">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="J6" t="s">
+        <v>57</v>
+      </c>
       <c r="K6">
         <v>1.22346697650319</v>
       </c>
@@ -743,7 +836,7 @@
         <v>1.18525751046228</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -756,6 +849,24 @@
       <c r="D7" t="s">
         <v>53</v>
       </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="G7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" t="s">
+        <v>57</v>
+      </c>
       <c r="K7">
         <v>1.1942316531331401</v>
       </c>
@@ -763,7 +874,7 @@
         <v>1.2281064586110499</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -776,6 +887,24 @@
       <c r="D8" t="s">
         <v>53</v>
       </c>
+      <c r="E8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="J8" t="s">
+        <v>57</v>
+      </c>
       <c r="K8">
         <v>4.3291891272365799</v>
       </c>
@@ -783,7 +912,7 @@
         <v>5.6191238974615096</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -796,6 +925,24 @@
       <c r="D9" t="s">
         <v>53</v>
       </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="H9">
+        <v>5.5899999999999998E-2</v>
+      </c>
+      <c r="I9">
+        <v>0.159</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
       <c r="K9">
         <v>1.6116152450090799</v>
       </c>
@@ -803,7 +950,7 @@
         <v>7.0701454234388299</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -823,7 +970,7 @@
         <v>1.44714318760121</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -836,6 +983,24 @@
       <c r="D11" t="s">
         <v>53</v>
       </c>
+      <c r="E11">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="F11">
+        <v>0.157</v>
+      </c>
+      <c r="G11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="I11">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="J11" t="s">
+        <v>57</v>
+      </c>
       <c r="K11">
         <v>1.2089874411303001</v>
       </c>
@@ -843,7 +1008,7 @@
         <v>13.5093457943925</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -863,7 +1028,7 @@
         <v>1.89681512397858</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -883,7 +1048,7 @@
         <v>2.1194152923538199</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -896,6 +1061,24 @@
       <c r="D14" t="s">
         <v>53</v>
       </c>
+      <c r="E14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14">
+        <v>0.224</v>
+      </c>
+      <c r="G14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14">
+        <v>0.126</v>
+      </c>
+      <c r="J14" t="s">
+        <v>57</v>
+      </c>
       <c r="K14">
         <v>5.3298717611009199</v>
       </c>
@@ -903,7 +1086,7 @@
         <v>1.8087005749491001</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -916,6 +1099,24 @@
       <c r="D15" t="s">
         <v>53</v>
       </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="G15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" t="s">
+        <v>57</v>
+      </c>
       <c r="K15">
         <v>4.28793576582986</v>
       </c>
@@ -923,7 +1124,7 @@
         <v>1.7123751901077799</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -936,6 +1137,24 @@
       <c r="D16" t="s">
         <v>53</v>
       </c>
+      <c r="E16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16">
+        <v>6.7699999999999996E-2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" t="s">
+        <v>57</v>
+      </c>
       <c r="K16">
         <v>2.5620418137388001</v>
       </c>
@@ -943,7 +1162,7 @@
         <v>1.9964657515806601</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -956,6 +1175,24 @@
       <c r="D17" t="s">
         <v>53</v>
       </c>
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17">
+        <v>0.19</v>
+      </c>
+      <c r="G17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" t="s">
+        <v>57</v>
+      </c>
       <c r="K17">
         <v>6.7014936924386603</v>
       </c>
@@ -963,7 +1200,7 @@
         <v>7.4328530259366001</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -976,6 +1213,24 @@
       <c r="D18" t="s">
         <v>53</v>
       </c>
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18">
+        <v>9.4600000000000004E-2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="J18" t="s">
+        <v>57</v>
+      </c>
       <c r="K18">
         <v>1.65638647516996</v>
       </c>
@@ -983,7 +1238,7 @@
         <v>0.99923999603476199</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -996,6 +1251,24 @@
       <c r="D19" t="s">
         <v>53</v>
       </c>
+      <c r="E19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="J19" t="s">
+        <v>57</v>
+      </c>
       <c r="K19">
         <v>1.37363055097277</v>
       </c>
@@ -1003,7 +1276,7 @@
         <v>1.9186171093514099</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1016,6 +1289,24 @@
       <c r="D20" t="s">
         <v>53</v>
       </c>
+      <c r="E20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20">
+        <v>0.37</v>
+      </c>
+      <c r="G20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20">
+        <v>2.1899999999999999E-2</v>
+      </c>
+      <c r="I20">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="J20" t="s">
+        <v>57</v>
+      </c>
       <c r="K20">
         <v>1.8177167080836101</v>
       </c>
@@ -1023,7 +1314,7 @@
         <v>1.4403063084964101</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1043,7 +1334,7 @@
         <v>1.55283307810107</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1063,7 +1354,7 @@
         <v>1.0608695652173901</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1083,7 +1374,7 @@
         <v>1.6482539682539701</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1103,7 +1394,7 @@
         <v>1.8551042081508</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1123,7 +1414,7 @@
         <v>1.71892001258936</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1143,7 +1434,7 @@
         <v>2.9428263214671002</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1163,7 +1454,7 @@
         <v>1.7157821652348699</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1183,7 +1474,7 @@
         <v>2.9978270317253402</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1203,7 +1494,7 @@
         <v>2.0433168316831698</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1223,7 +1514,7 @@
         <v>2.93520746744323</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1243,7 +1534,7 @@
         <v>1.5907014295639901</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1263,7 +1554,7 @@
         <v>1.3730807932581399</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1283,7 +1574,7 @@
         <v>71.726027397260296</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1303,7 +1594,7 @@
         <v>3.1600621600621599</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1323,7 +1614,7 @@
         <v>1.6942884909065701</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -1343,7 +1634,7 @@
         <v>15.125</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1363,7 +1654,7 @@
         <v>52.941176470588204</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -1383,7 +1674,7 @@
         <v>24.439393939393899</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -1403,7 +1694,7 @@
         <v>88.749999999999901</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -1423,7 +1714,7 @@
         <v>2.3263157894736901</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -1443,7 +1734,7 @@
         <v>0.89644746787604002</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -1463,7 +1754,7 @@
         <v>4.1333333333333302</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -1483,7 +1774,7 @@
         <v>2.45875622085505</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
added all p values
</commit_message>
<xml_diff>
--- a/output/bigexcel.xlsx
+++ b/output/bigexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saqin\Desktop\Something_Cool-CpG_Sites-\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7D1CB2-0788-49A5-9DE6-9B18DF9F3D99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D810D4F-F737-4DDE-924A-7019539459EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4215" yWindow="465" windowWidth="27645" windowHeight="15960" xr2:uid="{8D3C0EB5-B848-6042-B945-4E985C0A2D75}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="58">
   <si>
     <t>File</t>
   </si>
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFE611C-6421-1741-B53C-4075AD299B10}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -961,7 +961,25 @@
         <v>864</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="E10">
+        <v>0.624</v>
+      </c>
+      <c r="F10">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="G10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>57</v>
       </c>
       <c r="K10">
         <v>0.55469924812030103</v>
@@ -1021,6 +1039,24 @@
       <c r="D12" t="s">
         <v>54</v>
       </c>
+      <c r="E12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12">
+        <v>6.6400000000000001E-2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12">
+        <v>0.35</v>
+      </c>
+      <c r="J12" t="s">
+        <v>57</v>
+      </c>
       <c r="K12">
         <v>0.95629383063770501</v>
       </c>
@@ -1041,6 +1077,24 @@
       <c r="D13" t="s">
         <v>54</v>
       </c>
+      <c r="E13">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="F13">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="G13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13">
+        <v>0.129</v>
+      </c>
+      <c r="J13" t="s">
+        <v>57</v>
+      </c>
       <c r="K13">
         <v>0.65142857142857202</v>
       </c>
@@ -1327,6 +1381,24 @@
       <c r="D21" t="s">
         <v>53</v>
       </c>
+      <c r="E21">
+        <v>7.8299999999999995E-2</v>
+      </c>
+      <c r="F21">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="G21" t="s">
+        <v>57</v>
+      </c>
+      <c r="H21">
+        <v>8.4699999999999998E-2</v>
+      </c>
+      <c r="I21">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="J21" t="s">
+        <v>57</v>
+      </c>
       <c r="K21">
         <v>1.87974683544304</v>
       </c>
@@ -1347,6 +1419,24 @@
       <c r="D22" t="s">
         <v>53</v>
       </c>
+      <c r="E22">
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="F22">
+        <v>0.625</v>
+      </c>
+      <c r="G22" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="I22">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="J22" t="s">
+        <v>57</v>
+      </c>
       <c r="K22">
         <v>1.68548284219926</v>
       </c>
@@ -1367,6 +1457,24 @@
       <c r="D23" t="s">
         <v>54</v>
       </c>
+      <c r="E23">
+        <v>3.3599999999999998E-2</v>
+      </c>
+      <c r="F23">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="G23" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23">
+        <v>0.02</v>
+      </c>
+      <c r="I23">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="J23" t="s">
+        <v>57</v>
+      </c>
       <c r="K23">
         <v>1.9529602595296001</v>
       </c>
@@ -1387,6 +1495,24 @@
       <c r="D24" t="s">
         <v>53</v>
       </c>
+      <c r="E24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="G24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24">
+        <v>2.4400000000000002E-2</v>
+      </c>
+      <c r="I24">
+        <v>0.126</v>
+      </c>
+      <c r="J24" t="s">
+        <v>57</v>
+      </c>
       <c r="K24">
         <v>1.68513274613182</v>
       </c>
@@ -1407,6 +1533,24 @@
       <c r="D25" t="s">
         <v>53</v>
       </c>
+      <c r="E25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="G25" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" t="s">
+        <v>57</v>
+      </c>
+      <c r="I25">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="J25" t="s">
+        <v>57</v>
+      </c>
       <c r="K25">
         <v>2.0858316988885801</v>
       </c>
@@ -1427,6 +1571,24 @@
       <c r="D26" t="s">
         <v>53</v>
       </c>
+      <c r="E26">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="F26">
+        <v>0.12</v>
+      </c>
+      <c r="G26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="J26" t="s">
+        <v>57</v>
+      </c>
       <c r="K26">
         <v>2.08587257617729</v>
       </c>
@@ -1447,6 +1609,24 @@
       <c r="D27" t="s">
         <v>54</v>
       </c>
+      <c r="E27">
+        <v>1.15E-2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="H27">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="I27" t="s">
+        <v>57</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
       <c r="K27">
         <v>2.4017109777862702</v>
       </c>
@@ -1467,6 +1647,24 @@
       <c r="D28" t="s">
         <v>53</v>
       </c>
+      <c r="E28" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="I28" t="s">
+        <v>57</v>
+      </c>
+      <c r="J28" t="s">
+        <v>57</v>
+      </c>
       <c r="K28">
         <v>1.55874086565486</v>
       </c>
@@ -1487,6 +1685,24 @@
       <c r="D29" t="s">
         <v>53</v>
       </c>
+      <c r="E29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29">
+        <v>0.193</v>
+      </c>
+      <c r="G29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29" t="s">
+        <v>57</v>
+      </c>
+      <c r="I29">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="J29" t="s">
+        <v>57</v>
+      </c>
       <c r="K29">
         <v>1.45734569689945</v>
       </c>
@@ -1507,6 +1723,24 @@
       <c r="D30" t="s">
         <v>53</v>
       </c>
+      <c r="E30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" t="s">
+        <v>57</v>
+      </c>
+      <c r="H30" t="s">
+        <v>57</v>
+      </c>
+      <c r="I30">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="J30" t="s">
+        <v>57</v>
+      </c>
       <c r="K30">
         <v>6.0309845124426698</v>
       </c>
@@ -1527,6 +1761,24 @@
       <c r="D31" t="s">
         <v>54</v>
       </c>
+      <c r="E31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31">
+        <v>8.5199999999999998E-2</v>
+      </c>
+      <c r="H31">
+        <v>6.9500000000000006E-2</v>
+      </c>
+      <c r="I31">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="J31">
+        <v>0.23699999999999999</v>
+      </c>
       <c r="K31">
         <v>2.3982939632545901</v>
       </c>
@@ -1547,6 +1799,24 @@
       <c r="D32" t="s">
         <v>53</v>
       </c>
+      <c r="E32">
+        <v>1.03E-2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="I32">
+        <v>6.7799999999999999E-2</v>
+      </c>
+      <c r="J32" t="s">
+        <v>57</v>
+      </c>
       <c r="K32">
         <v>1.78218357932643</v>
       </c>
@@ -1565,7 +1835,25 @@
         <v>1086</v>
       </c>
       <c r="D33" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="E33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33">
+        <v>0.43</v>
+      </c>
+      <c r="G33" t="s">
+        <v>57</v>
+      </c>
+      <c r="H33" t="s">
+        <v>57</v>
+      </c>
+      <c r="I33">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="J33" t="s">
+        <v>57</v>
       </c>
       <c r="K33">
         <v>62.922619047619101</v>
@@ -1587,6 +1875,24 @@
       <c r="D34" t="s">
         <v>53</v>
       </c>
+      <c r="E34">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="F34">
+        <v>8.7300000000000003E-2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>57</v>
+      </c>
+      <c r="H34">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="I34">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="J34" t="s">
+        <v>57</v>
+      </c>
       <c r="K34">
         <v>16.051724137931</v>
       </c>
@@ -1607,6 +1913,24 @@
       <c r="D35" t="s">
         <v>53</v>
       </c>
+      <c r="E35">
+        <v>3.3500000000000002E-2</v>
+      </c>
+      <c r="F35">
+        <v>0.93</v>
+      </c>
+      <c r="G35" t="s">
+        <v>57</v>
+      </c>
+      <c r="H35">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="I35" t="s">
+        <v>57</v>
+      </c>
+      <c r="J35" t="s">
+        <v>57</v>
+      </c>
       <c r="K35">
         <v>2.6267006802721098</v>
       </c>
@@ -1627,6 +1951,24 @@
       <c r="D36" t="s">
         <v>53</v>
       </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="G36">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="H36">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="I36">
+        <v>0.316</v>
+      </c>
+      <c r="J36">
+        <v>0.17499999999999999</v>
+      </c>
       <c r="K36">
         <v>0.33333333333333298</v>
       </c>
@@ -1647,6 +1989,24 @@
       <c r="D37" t="s">
         <v>54</v>
       </c>
+      <c r="E37">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="F37">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="G37">
+        <v>0.85</v>
+      </c>
+      <c r="H37">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="I37">
+        <v>2.7699999999999999E-2</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
       <c r="K37">
         <v>126.578947368421</v>
       </c>
@@ -1667,6 +2027,24 @@
       <c r="D38" t="s">
         <v>53</v>
       </c>
+      <c r="E38">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="F38">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="G38" t="s">
+        <v>57</v>
+      </c>
+      <c r="H38">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="I38">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="J38" t="s">
+        <v>57</v>
+      </c>
       <c r="K38">
         <v>0.95887047268262604</v>
       </c>
@@ -1687,6 +2065,24 @@
       <c r="D39" t="s">
         <v>53</v>
       </c>
+      <c r="E39">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="F39">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="G39">
+        <v>0.441</v>
+      </c>
+      <c r="H39">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="I39">
+        <v>7.3300000000000004E-2</v>
+      </c>
+      <c r="J39">
+        <v>0.83799999999999997</v>
+      </c>
       <c r="K39">
         <v>18.952380952380899</v>
       </c>
@@ -1707,6 +2103,24 @@
       <c r="D40" t="s">
         <v>53</v>
       </c>
+      <c r="E40">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="F40">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="G40">
+        <v>0.249</v>
+      </c>
+      <c r="H40">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="I40">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="J40">
+        <v>0.46600000000000003</v>
+      </c>
       <c r="K40">
         <v>2.3547794117647101</v>
       </c>
@@ -1727,6 +2141,24 @@
       <c r="D41" t="s">
         <v>53</v>
       </c>
+      <c r="E41">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="F41">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="G41">
+        <v>9.0499999999999997E-2</v>
+      </c>
+      <c r="H41">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="I41">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="J41">
+        <v>0.54400000000000004</v>
+      </c>
       <c r="K41">
         <v>1.0212765957446801</v>
       </c>
@@ -1747,6 +2179,24 @@
       <c r="D42" t="s">
         <v>53</v>
       </c>
+      <c r="E42">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="F42">
+        <v>3.2099999999999997E-2</v>
+      </c>
+      <c r="G42">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="H42">
+        <v>0.21</v>
+      </c>
+      <c r="I42">
+        <v>4.8300000000000003E-2</v>
+      </c>
+      <c r="J42">
+        <v>0.74199999999999999</v>
+      </c>
       <c r="K42">
         <v>6.6666666666666696</v>
       </c>
@@ -1767,6 +2217,24 @@
       <c r="D43" t="s">
         <v>53</v>
       </c>
+      <c r="E43" t="s">
+        <v>57</v>
+      </c>
+      <c r="F43">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="G43" t="s">
+        <v>57</v>
+      </c>
+      <c r="H43" t="s">
+        <v>57</v>
+      </c>
+      <c r="I43">
+        <v>0.308</v>
+      </c>
+      <c r="J43" t="s">
+        <v>57</v>
+      </c>
       <c r="K43">
         <v>2.7296605668485299</v>
       </c>
@@ -1786,6 +2254,24 @@
       </c>
       <c r="D44" t="s">
         <v>53</v>
+      </c>
+      <c r="E44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F44">
+        <v>0.755</v>
+      </c>
+      <c r="G44" t="s">
+        <v>57</v>
+      </c>
+      <c r="H44" t="s">
+        <v>57</v>
+      </c>
+      <c r="I44">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="J44" t="s">
+        <v>57</v>
       </c>
       <c r="K44">
         <v>3.20552027629234</v>

</xml_diff>

<commit_message>
added which database viruses came from
</commit_message>
<xml_diff>
--- a/output/bigexcel.xlsx
+++ b/output/bigexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saqin\Desktop\Something_Cool-CpG_Sites-\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D810D4F-F737-4DDE-924A-7019539459EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF183CE-5383-47F5-8E10-DB53145F25A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4215" yWindow="465" windowWidth="27645" windowHeight="15960" xr2:uid="{8D3C0EB5-B848-6042-B945-4E985C0A2D75}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="61">
   <si>
     <t>File</t>
   </si>
@@ -220,12 +220,6 @@
     <t>T-&gt;C Syn v NonSyn</t>
   </si>
   <si>
-    <t>Data 2019</t>
-  </si>
-  <si>
-    <t>NESCENT</t>
-  </si>
-  <si>
     <t>Costly: A-&gt;G Syn</t>
   </si>
   <si>
@@ -233,6 +227,21 @@
   </si>
   <si>
     <t>&lt;0.01</t>
+  </si>
+  <si>
+    <t>HIV Database</t>
+  </si>
+  <si>
+    <t>Virus Pathogen Resource</t>
+  </si>
+  <si>
+    <t>NCBI GenBank 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GenBank </t>
+  </si>
+  <si>
+    <t>GenBank</t>
   </si>
 </sst>
 </file>
@@ -599,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFE611C-6421-1741-B53C-4075AD299B10}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -640,10 +649,10 @@
         <v>52</v>
       </c>
       <c r="K1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -657,25 +666,25 @@
         <v>10176</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K2">
         <v>2.2271225403678701</v>
@@ -695,25 +704,25 @@
         <v>10173</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I3">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="J3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K3">
         <v>1.38769839128198</v>
@@ -733,25 +742,25 @@
         <v>10170</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F4">
         <v>2.2700000000000001E-2</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K4">
         <v>1.69459448388228</v>
@@ -771,25 +780,25 @@
         <v>10206</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F5">
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K5">
         <v>1.90734628459693</v>
@@ -809,7 +818,7 @@
         <v>9036</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E6">
         <v>2.1600000000000001E-2</v>
@@ -818,7 +827,7 @@
         <v>0.38200000000000001</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H6">
         <v>2.3699999999999999E-2</v>
@@ -827,7 +836,7 @@
         <v>0.19800000000000001</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K6">
         <v>1.22346697650319</v>
@@ -847,25 +856,25 @@
         <v>9036</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F7">
         <v>0.88300000000000001</v>
       </c>
       <c r="G7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K7">
         <v>1.1942316531331401</v>
@@ -885,25 +894,25 @@
         <v>3264</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I8">
         <v>0.16300000000000001</v>
       </c>
       <c r="J8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K8">
         <v>4.3291891272365799</v>
@@ -923,13 +932,13 @@
         <v>1782</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G9">
         <v>0.98799999999999999</v>
@@ -961,7 +970,7 @@
         <v>864</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E10">
         <v>0.624</v>
@@ -970,7 +979,7 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H10">
         <v>1.7600000000000001E-2</v>
@@ -979,7 +988,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K10">
         <v>0.55469924812030103</v>
@@ -999,7 +1008,7 @@
         <v>1716</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E11">
         <v>0.10299999999999999</v>
@@ -1008,7 +1017,7 @@
         <v>0.157</v>
       </c>
       <c r="G11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H11">
         <v>7.7200000000000005E-2</v>
@@ -1017,7 +1026,7 @@
         <v>0.13900000000000001</v>
       </c>
       <c r="J11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K11">
         <v>1.2089874411303001</v>
@@ -1037,25 +1046,25 @@
         <v>15471</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F12">
         <v>6.6400000000000001E-2</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I12">
         <v>0.35</v>
       </c>
       <c r="J12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K12">
         <v>0.95629383063770501</v>
@@ -1075,7 +1084,7 @@
         <v>1617</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E13">
         <v>0.77700000000000002</v>
@@ -1084,16 +1093,16 @@
         <v>0.29799999999999999</v>
       </c>
       <c r="G13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I13">
         <v>0.129</v>
       </c>
       <c r="J13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K13">
         <v>0.65142857142857202</v>
@@ -1113,25 +1122,25 @@
         <v>1407</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F14">
         <v>0.224</v>
       </c>
       <c r="G14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I14">
         <v>0.126</v>
       </c>
       <c r="J14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K14">
         <v>5.3298717611009199</v>
@@ -1151,25 +1160,25 @@
         <v>1710</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F15">
         <v>0.38500000000000001</v>
       </c>
       <c r="G15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K15">
         <v>4.28793576582986</v>
@@ -1189,25 +1198,25 @@
         <v>1701</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F16">
         <v>6.7699999999999996E-2</v>
       </c>
       <c r="G16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K16">
         <v>2.5620418137388001</v>
@@ -1227,25 +1236,25 @@
         <v>1410</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F17">
         <v>0.19</v>
       </c>
       <c r="G17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K17">
         <v>6.7014936924386603</v>
@@ -1265,25 +1274,25 @@
         <v>1755</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F18">
         <v>9.4600000000000004E-2</v>
       </c>
       <c r="G18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I18">
         <v>0.16200000000000001</v>
       </c>
       <c r="J18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K18">
         <v>1.65638647516996</v>
@@ -1303,25 +1312,25 @@
         <v>1398</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F19">
         <v>3.2800000000000003E-2</v>
       </c>
       <c r="G19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I19">
         <v>0.23699999999999999</v>
       </c>
       <c r="J19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K19">
         <v>1.37363055097277</v>
@@ -1341,16 +1350,16 @@
         <v>894</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F20">
         <v>0.37</v>
       </c>
       <c r="G20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H20">
         <v>2.1899999999999999E-2</v>
@@ -1359,7 +1368,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="J20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K20">
         <v>1.8177167080836101</v>
@@ -1379,7 +1388,7 @@
         <v>294</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E21">
         <v>7.8299999999999995E-2</v>
@@ -1388,7 +1397,7 @@
         <v>0.47699999999999998</v>
       </c>
       <c r="G21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H21">
         <v>8.4699999999999998E-2</v>
@@ -1397,7 +1406,7 @@
         <v>0.54500000000000004</v>
       </c>
       <c r="J21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K21">
         <v>1.87974683544304</v>
@@ -1417,7 +1426,7 @@
         <v>876</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E22">
         <v>2.5600000000000001E-2</v>
@@ -1426,7 +1435,7 @@
         <v>0.625</v>
       </c>
       <c r="G22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H22">
         <v>0.40699999999999997</v>
@@ -1435,7 +1444,7 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="J22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K22">
         <v>1.68548284219926</v>
@@ -1455,7 +1464,7 @@
         <v>283</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E23">
         <v>3.3599999999999998E-2</v>
@@ -1464,7 +1473,7 @@
         <v>0.56699999999999995</v>
       </c>
       <c r="G23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H23">
         <v>0.02</v>
@@ -1473,7 +1482,7 @@
         <v>0.17699999999999999</v>
       </c>
       <c r="J23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K23">
         <v>1.9529602595296001</v>
@@ -1493,16 +1502,16 @@
         <v>906</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F24">
         <v>0.28799999999999998</v>
       </c>
       <c r="G24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H24">
         <v>2.4400000000000002E-2</v>
@@ -1511,7 +1520,7 @@
         <v>0.126</v>
       </c>
       <c r="J24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K24">
         <v>1.68513274613182</v>
@@ -1531,25 +1540,25 @@
         <v>813</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F25">
         <v>0.92600000000000005</v>
       </c>
       <c r="G25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I25">
         <v>0.48799999999999999</v>
       </c>
       <c r="J25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K25">
         <v>2.0858316988885801</v>
@@ -1569,7 +1578,7 @@
         <v>528</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E26">
         <v>1.5800000000000002E-2</v>
@@ -1578,16 +1587,16 @@
         <v>0.12</v>
       </c>
       <c r="G26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I26">
         <v>0.89700000000000002</v>
       </c>
       <c r="J26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K26">
         <v>2.08587257617729</v>
@@ -1607,13 +1616,13 @@
         <v>15132</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E27">
         <v>1.15E-2</v>
       </c>
       <c r="F27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G27">
         <v>0.88100000000000001</v>
@@ -1622,7 +1631,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
       <c r="I27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -1645,25 +1654,25 @@
         <v>900</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F28">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="G28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H28">
         <v>0.14299999999999999</v>
       </c>
       <c r="I28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K28">
         <v>1.55874086565486</v>
@@ -1683,25 +1692,25 @@
         <v>1851</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F29">
         <v>0.193</v>
       </c>
       <c r="G29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I29">
         <v>1.7399999999999999E-2</v>
       </c>
       <c r="J29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K29">
         <v>1.45734569689945</v>
@@ -1721,25 +1730,25 @@
         <v>6579</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I30">
         <v>4.2599999999999999E-2</v>
       </c>
       <c r="J30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K30">
         <v>6.0309845124426698</v>
@@ -1759,13 +1768,13 @@
         <v>6933</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G31">
         <v>8.5199999999999998E-2</v>
@@ -1797,16 +1806,16 @@
         <v>1197</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E32">
         <v>1.03E-2</v>
       </c>
       <c r="F32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H32">
         <v>2.1100000000000001E-2</v>
@@ -1815,7 +1824,7 @@
         <v>6.7799999999999999E-2</v>
       </c>
       <c r="J32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K32">
         <v>1.78218357932643</v>
@@ -1835,25 +1844,25 @@
         <v>1086</v>
       </c>
       <c r="D33" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F33">
         <v>0.43</v>
       </c>
       <c r="G33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I33">
         <v>0.93899999999999995</v>
       </c>
       <c r="J33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K33">
         <v>62.922619047619101</v>
@@ -1873,7 +1882,7 @@
         <v>2013</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E34">
         <v>0.19500000000000001</v>
@@ -1882,7 +1891,7 @@
         <v>8.7300000000000003E-2</v>
       </c>
       <c r="G34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H34">
         <v>0.25800000000000001</v>
@@ -1891,7 +1900,7 @@
         <v>0.14099999999999999</v>
       </c>
       <c r="J34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K34">
         <v>16.051724137931</v>
@@ -1911,7 +1920,7 @@
         <v>1620</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E35">
         <v>3.3500000000000002E-2</v>
@@ -1920,16 +1929,16 @@
         <v>0.93</v>
       </c>
       <c r="G35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H35">
         <v>4.3299999999999998E-2</v>
       </c>
       <c r="I35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K35">
         <v>2.6267006802721098</v>
@@ -1949,7 +1958,7 @@
         <v>251</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1987,7 +1996,7 @@
         <v>181</v>
       </c>
       <c r="D37" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E37">
         <v>0.23200000000000001</v>
@@ -2025,7 +2034,7 @@
         <v>264</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E38">
         <v>0.59299999999999997</v>
@@ -2034,7 +2043,7 @@
         <v>0.79800000000000004</v>
       </c>
       <c r="G38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H38">
         <v>0.49199999999999999</v>
@@ -2043,7 +2052,7 @@
         <v>0.69199999999999995</v>
       </c>
       <c r="J38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K38">
         <v>0.95887047268262604</v>
@@ -2063,7 +2072,7 @@
         <v>678</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E39">
         <v>0.61599999999999999</v>
@@ -2101,7 +2110,7 @@
         <v>462</v>
       </c>
       <c r="D40" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E40">
         <v>0.22600000000000001</v>
@@ -2139,7 +2148,7 @@
         <v>1317</v>
       </c>
       <c r="D41" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E41">
         <v>0.39800000000000002</v>
@@ -2177,7 +2186,7 @@
         <v>1458</v>
       </c>
       <c r="D42" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E42">
         <v>0.36099999999999999</v>
@@ -2215,25 +2224,25 @@
         <v>2016</v>
       </c>
       <c r="D43" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F43">
         <v>0.76300000000000001</v>
       </c>
       <c r="G43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I43">
         <v>0.308</v>
       </c>
       <c r="J43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K43">
         <v>2.7296605668485299</v>
@@ -2253,25 +2262,25 @@
         <v>2343</v>
       </c>
       <c r="D44" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F44">
         <v>0.755</v>
       </c>
       <c r="G44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I44">
         <v>0.80100000000000005</v>
       </c>
       <c r="J44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K44">
         <v>3.20552027629234</v>

</xml_diff>